<commit_message>
Updated Passwords to include FTP
ftp.womencoders.org
</commit_message>
<xml_diff>
--- a/WOMENCODER-copy/Usernamepasswords.xlsx
+++ b/WOMENCODER-copy/Usernamepasswords.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Women-Coders\WOMENCODER-copy\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +54,12 @@
   </si>
   <si>
     <t>Gmail</t>
+  </si>
+  <si>
+    <t>FTP Server</t>
+  </si>
+  <si>
+    <t>peoplespace88</t>
   </si>
 </sst>
 </file>
@@ -116,6 +127,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -163,7 +177,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -198,7 +212,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -407,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,9 +434,10 @@
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -438,8 +453,11 @@
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -455,8 +473,11 @@
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -471,6 +492,9 @@
       </c>
       <c r="E3" t="s">
         <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added password and artwork
password for sprite. Logo files for t-shirt
</commit_message>
<xml_diff>
--- a/WOMENCODER-copy/Usernamepasswords.xlsx
+++ b/WOMENCODER-copy/Usernamepasswords.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>peoplespace88</t>
+  </si>
+  <si>
+    <t>Stripe</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,9 +438,10 @@
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -456,8 +460,11 @@
       <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -476,8 +483,11 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -495,14 +505,18 @@
       </c>
       <c r="F3" t="s">
         <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated username and passwords
updated
</commit_message>
<xml_diff>
--- a/WOMENCODER-copy/Usernamepasswords.xlsx
+++ b/WOMENCODER-copy/Usernamepasswords.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Women-Coders\WOMENCODER-copy\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -60,6 +55,18 @@
   </si>
   <si>
     <t>peoplespace88</t>
+  </si>
+  <si>
+    <t>Stripe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">womencoders@gmail.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">host </t>
+  </si>
+  <si>
+    <t>ftp.womencoders.org</t>
   </si>
 </sst>
 </file>
@@ -177,7 +184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,7 +219,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -421,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,10 +441,11 @@
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -456,8 +464,11 @@
       <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -476,8 +487,11 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -495,14 +509,29 @@
       </c>
       <c r="F3" t="s">
         <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="F6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>